<commit_message>
Completed Week 2 Challenges and Assessment
</commit_message>
<xml_diff>
--- a/Excel Calculations W02_Challenge01.xlsx
+++ b/Excel Calculations W02_Challenge01.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA ANALYSIS AND DATA SCIENCE PROJECTS\Excel Skills for Business Essentials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD495DAC-B8D4-42CD-AE7A-F6589EFBA07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF70CAD6-FD50-48BF-BEC5-6018D1AA92AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Title page" sheetId="4" r:id="rId1"/>
     <sheet name="Trip Costs" sheetId="2" r:id="rId2"/>
     <sheet name="Payments" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -869,7 +869,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:O6"/>
+      <selection activeCell="A12" sqref="A12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1141,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1194,7 +1194,10 @@
         <v>210</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="D6" s="5">
+        <f>B6*$B$3</f>
+        <v>2520</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
@@ -1206,7 +1209,10 @@
       <c r="C7" s="5">
         <v>1</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="5">
+        <f>B7*C7</f>
+        <v>375</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
@@ -1216,7 +1222,10 @@
         <v>75</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="D8" s="5">
+        <f t="shared" ref="D7:D11" si="0">B8*$B$3</f>
+        <v>900</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
@@ -1226,7 +1235,10 @@
         <v>6.5</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
@@ -1236,7 +1248,10 @@
         <v>21.5</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
@@ -1248,7 +1263,10 @@
       <c r="C11" s="5">
         <v>1</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="5">
+        <f>B11*C11</f>
+        <v>69</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15" thickBot="1">
       <c r="A12" s="4" t="s">
@@ -1256,14 +1274,20 @@
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4">
+        <f>SUM(D6:D11)</f>
+        <v>4200</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="15" thickTop="1"/>
     <row r="14" spans="1:4">
       <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="8">
+        <f>D12/B3</f>
+        <v>350</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D14">
@@ -1272,6 +1296,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D7" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1279,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1345,6 +1372,14 @@
       <c r="F4">
         <v>150</v>
       </c>
+      <c r="G4">
+        <f>SUM(D4:F4)</f>
+        <v>350</v>
+      </c>
+      <c r="H4">
+        <f>C4-G4</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
@@ -1365,6 +1400,14 @@
       <c r="F5">
         <v>0</v>
       </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G15" si="0">SUM(D5:F5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H15" si="1">C5-G5</f>
+        <v>350</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -1385,6 +1428,14 @@
       <c r="F6">
         <v>0</v>
       </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>170</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -1405,6 +1456,14 @@
       <c r="F7">
         <v>0</v>
       </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -1425,6 +1484,14 @@
       <c r="F8">
         <v>150</v>
       </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -1445,6 +1512,14 @@
       <c r="F9">
         <v>0</v>
       </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -1465,6 +1540,14 @@
       <c r="F10">
         <v>0</v>
       </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -1485,6 +1568,14 @@
       <c r="F11">
         <v>0</v>
       </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -1505,6 +1596,14 @@
       <c r="F12">
         <v>0</v>
       </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -1525,6 +1624,14 @@
       <c r="F13">
         <v>0</v>
       </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -1545,6 +1652,14 @@
       <c r="F14">
         <v>150</v>
       </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -1565,21 +1680,41 @@
       <c r="F15">
         <v>0</v>
       </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4">
+        <f>SUM(C4:C15)</f>
+        <v>4200</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="G16" s="4">
+        <f>SUM(G4:G15)</f>
+        <v>2430</v>
+      </c>
+      <c r="H16" s="4">
+        <f>SUM(H4:H15)</f>
+        <v>1770</v>
+      </c>
     </row>
     <row r="17" ht="15" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="G4:G15" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>